<commit_message>
Cleanup section import.  Issue #42732
git-svn-id: svn+ssh://billy.knut.univention.de/var/univention/svn/dev/branches/ucs-4.1/ucs-school-4.1r2@78414 1b283449-9f2f-0410-b571-8eb228e1a901
</commit_message>
<xml_diff>
--- a/doc/manual/ucsschool-import-vorlagen.xlsx
+++ b/doc/manual/ucsschool-import-vorlagen.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Schulen" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Netzwerke" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Clients" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Netze" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Rechner" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Drucker" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Bentuzer" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Benutzer" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Klassen" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -25,12 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
-  <si>
-    <t xml:space="preserve"># Script /usr/share/ucs-school-import/scripts/import_schools, siehe UCS@school Start Guide</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Schulkürzel</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+  <si>
+    <t xml:space="preserve"># Skript /usr/share/ucs-school-import/scripts/import_schools, siehe UCS@school Start Guide</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Schule / OU</t>
   </si>
   <si>
     <t xml:space="preserve">Schulname</t>
@@ -42,62 +42,19 @@
     <t xml:space="preserve">Server Verwaltung</t>
   </si>
   <si>
-    <t xml:space="preserve">011</t>
+    <t xml:space="preserve">g123m</t>
   </si>
   <si>
     <t xml:space="preserve">Grundschule Nord</t>
   </si>
   <si>
-    <t xml:space="preserve">sedu011-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sadm011-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grundschule West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sedu012-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sadm012-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berufsschule Tec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sedu042-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sadm042-01</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:network:import</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"># Schule / OU</t>
+    <t xml:space="preserve">sedug123m-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sadmg123m-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:network:import</t>
   </si>
   <si>
     <t xml:space="preserve">Netzwerk</t>
@@ -115,23 +72,19 @@
     <t xml:space="preserve">(WINS-Server)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:computers</t>
-    </r>
+    <t xml:space="preserve">10.0.5.0/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0.5.10-​10.0.5.140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0.5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Dokumentation https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:computers</t>
   </si>
   <si>
     <t xml:space="preserve"># Rechnertyp</t>
@@ -164,29 +117,16 @@
     <t xml:space="preserve">10:00:ee:ﬀ:cc:00</t>
   </si>
   <si>
-    <t xml:space="preserve">g123m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.0.5.5</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:printers</t>
-    </r>
+    <t xml:space="preserve">10.0.5.5/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR47110815-XA-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edukativ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Dokumentation https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:printers</t>
   </si>
   <si>
     <t xml:space="preserve"># Aktion</t>
@@ -210,51 +150,67 @@
     <t xml:space="preserve">socket://10.0.5.250:9100</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:importusers</t>
-    </r>
+    <t xml:space="preserve"># Dokumentation https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:importusers</t>
   </si>
   <si>
     <t xml:space="preserve">Benutzername</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:classes</t>
-    </r>
+    <t xml:space="preserve">Nachname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vorname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rechte (veraltet)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Mailadresse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lehrer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aktiv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitarbeiter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m.mustermann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mustermann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g123m-1A,g123m-1B, g123m-2A,g123m-4C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">m.musterm@beispiel.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Dokumentation https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:classes</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppen- / Klassenname</t>
   </si>
   <si>
     <t xml:space="preserve">(Beschreibung)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g123m-1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klasse 1A</t>
   </si>
 </sst>
 </file>
@@ -270,6 +226,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -291,6 +248,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -335,12 +293,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,28 +323,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -396,7 +358,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -407,34 +369,6 @@
       </c>
       <c r="D3" s="0" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -453,55 +387,75 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>17</v>
+      <c r="A1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>23</v>
+      <c r="F3" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:network:import" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:network:import"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:network:import" display="# https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:network:import"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -516,73 +470,79 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.484693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>24</v>
+      <c r="A1" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:computers" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:computers"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:computers" display="# Dokumentation https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:computers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -597,64 +557,65 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>37</v>
+      <c r="A1" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:printers" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:printers"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:printers" display="# Dokumentation https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:printers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -667,37 +628,105 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>45</v>
+      <c r="A1" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>46</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:importusers" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:importusers"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:importusers" display="# Dokumentation https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:importusers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -710,46 +739,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>47</v>
+      <c r="A1" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:classes" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:classes"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:classes" display="# Dokumentation https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:classes"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Bug #49319: ucsschool scenarios: Adjust ucsschool-import-vorlagen.xlsx document
</commit_message>
<xml_diff>
--- a/doc/manual/ucsschool-import-vorlagen.xlsx
+++ b/doc/manual/ucsschool-import-vorlagen.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Netzwerke" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Clients" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Drucker" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Bentuzer" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Benutzer" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Klassen" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -25,9 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
-  <si>
-    <t xml:space="preserve"># Script /usr/share/ucs-school-import/scripts/import_schools, siehe UCS@school Start Guide</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="104">
+  <si>
+    <t xml:space="preserve"># Script /usr/share/ucs-school-import/scripts/create_ou</t>
   </si>
   <si>
     <t xml:space="preserve"># Schulkürzel</t>
@@ -39,7 +39,7 @@
     <t xml:space="preserve">Server Pädagogik</t>
   </si>
   <si>
-    <t xml:space="preserve">Server Verwaltung</t>
+    <t xml:space="preserve">(Server Verwaltung)</t>
   </si>
   <si>
     <t xml:space="preserve">011</t>
@@ -48,10 +48,7 @@
     <t xml:space="preserve">Grundschule Nord</t>
   </si>
   <si>
-    <t xml:space="preserve">sedu011-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sadm011-01</t>
+    <t xml:space="preserve">sedu-011-01</t>
   </si>
   <si>
     <t xml:space="preserve">012</t>
@@ -60,10 +57,7 @@
     <t xml:space="preserve">Grundschule West</t>
   </si>
   <si>
-    <t xml:space="preserve">sedu012-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sadm012-01</t>
+    <t xml:space="preserve">sedu-012-01</t>
   </si>
   <si>
     <t xml:space="preserve">042</t>
@@ -72,29 +66,13 @@
     <t xml:space="preserve">Berufsschule Tec</t>
   </si>
   <si>
-    <t xml:space="preserve">sedu042-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sadm042-01</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:network:import</t>
-    </r>
+    <t xml:space="preserve">sedu-042-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sadm-042-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:schoolcreate:network:import</t>
   </si>
   <si>
     <t xml:space="preserve"># Schule / OU</t>
@@ -115,23 +93,94 @@
     <t xml:space="preserve">(WINS-Server)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:computers</t>
-    </r>
+    <t xml:space="preserve">10.1.0.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1.0.1-10.1.0.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1.0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.0.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.0.1-10.2.0.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.1.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.2.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.2.1-10.42.2.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.4.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.4.1-10.42.4.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.6.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.6.1-10.42.6.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.6.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.8.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.8.1-10.42.8.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.128.0/20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.128.100-10.42.143.250 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.128.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.192.0/20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.192.100-10.42.207.250 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.192.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:schoolcreate:computers</t>
   </si>
   <si>
     <t xml:space="preserve"># Rechnertyp</t>
@@ -158,35 +207,19 @@
     <t xml:space="preserve">windows</t>
   </si>
   <si>
-    <t xml:space="preserve">wing123m-01</t>
+    <t xml:space="preserve">win-042-001 </t>
   </si>
   <si>
     <t xml:space="preserve">10:00:ee:ﬀ:cc:00</t>
   </si>
   <si>
-    <t xml:space="preserve">g123m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.0.5.5</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:printers</t>
-    </r>
+    <t xml:space="preserve">123-456-789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edukativ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:printers</t>
   </si>
   <si>
     <t xml:space="preserve"># Aktion</t>
@@ -201,54 +234,103 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">dcg123m-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g123m-laserdrucker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">socket://10.0.5.250:9100</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:importusers</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Benutzername</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:classes</t>
-    </r>
+    <t xml:space="preserve">dru-042-012 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket://10.42.1.201:9100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:importusers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Vorname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nachname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schulen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somerville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">042-7a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e7c66ffb-afe1-4290-88df-948821b24876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mary@example.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lovelace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">042-6b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b998acd3-774c-4ccd-97b7-5fec820cc9c4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ada@example.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Susan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">042-5c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8ccc861f-652e-4f96-b796-aea2a7e827c8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skare@example.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margaret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamilton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a2eaab3f-e034-4df5-b66b-4610d24596d3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nasa@moon.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hopper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1ad9f83a-3473-41e3-9bb7-32af7ba74983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grace@hopper.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:classes</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppen- / Klassenname</t>
@@ -270,6 +352,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -291,6 +374,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -335,7 +419,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,36 +428,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.97"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,36 +496,30 @@
       <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -449,59 +534,229 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>17</v>
+      <c r="A1" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:network:import" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:network:import"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:network:import" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:schoolcreate:network:import"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -510,79 +765,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.484693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>24</v>
+      <c r="A1" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>36</v>
+      <c r="F3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:computers" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:computers"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:computers" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:schoolcreate:computers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -591,70 +850,68 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>37</v>
+      <c r="A1" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>35</v>
+        <v>68</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>43</v>
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:printers" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:printers"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:printers" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:printers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -663,41 +920,154 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>45</v>
+      <c r="A1" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>73</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:importusers" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:importusers"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:importusers" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:importusers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -706,50 +1076,48 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>47</v>
+      <c r="A1" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:classes" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:classes"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:classes" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:classes"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Bug #49319: ucsschool scenarios: Minor Fix to screenshot and template
</commit_message>
<xml_diff>
--- a/doc/manual/ucsschool-import-vorlagen.xlsx
+++ b/doc/manual/ucsschool-import-vorlagen.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
   <si>
     <t xml:space="preserve"># Script /usr/share/ucs-school-import/scripts/create_ou</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t xml:space="preserve">(Server Verwaltung)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Server Fileshares)</t>
   </si>
   <si>
     <t xml:space="preserve">011</t>
@@ -453,18 +456,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,41 +489,44 @@
       <c r="D2" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +551,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.88"/>
@@ -555,199 +562,199 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -775,64 +782,64 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -860,49 +867,49 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -930,135 +937,135 @@
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1086,29 +1093,29 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug #54392: Update the import template from bug #49319
</commit_message>
<xml_diff>
--- a/doc/manual/ucsschool-import-vorlagen.xlsx
+++ b/doc/manual/ucsschool-import-vorlagen.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Netzwerke" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Clients" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Drucker" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Bentuzer" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Benutzer" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Klassen" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -25,9 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
-  <si>
-    <t xml:space="preserve"># Script /usr/share/ucs-school-import/scripts/import_schools, siehe UCS@school Start Guide</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
+  <si>
+    <t xml:space="preserve"># Script /usr/share/ucs-school-import/scripts/create_ou</t>
   </si>
   <si>
     <t xml:space="preserve"># Schulkürzel</t>
@@ -39,7 +39,10 @@
     <t xml:space="preserve">Server Pädagogik</t>
   </si>
   <si>
-    <t xml:space="preserve">Server Verwaltung</t>
+    <t xml:space="preserve">(Server Verwaltung)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Server Fileshares)</t>
   </si>
   <si>
     <t xml:space="preserve">011</t>
@@ -48,10 +51,7 @@
     <t xml:space="preserve">Grundschule Nord</t>
   </si>
   <si>
-    <t xml:space="preserve">sedu011-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sadm011-01</t>
+    <t xml:space="preserve">sedu-011-01</t>
   </si>
   <si>
     <t xml:space="preserve">012</t>
@@ -60,10 +60,7 @@
     <t xml:space="preserve">Grundschule West</t>
   </si>
   <si>
-    <t xml:space="preserve">sedu012-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sadm012-01</t>
+    <t xml:space="preserve">sedu-012-01</t>
   </si>
   <si>
     <t xml:space="preserve">042</t>
@@ -72,29 +69,13 @@
     <t xml:space="preserve">Berufsschule Tec</t>
   </si>
   <si>
-    <t xml:space="preserve">sedu042-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sadm042-01</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:network:import</t>
-    </r>
+    <t xml:space="preserve">sedu-042-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sadm-042-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:schoolcreate:network:import</t>
   </si>
   <si>
     <t xml:space="preserve"># Schule / OU</t>
@@ -115,23 +96,94 @@
     <t xml:space="preserve">(WINS-Server)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:computers</t>
-    </r>
+    <t xml:space="preserve">10.1.0.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1.0.1-10.1.0.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1.0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.0.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.0.1-10.2.0.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.1.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.2.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.2.1-10.42.2.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.4.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.4.1-10.42.4.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.6.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.6.1-10.42.6.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.6.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.8.0/24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.8.1-10.42.8.254 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.128.0/20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.128.100-10.42.143.250 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.128.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.192.0/20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.192.100-10.42.207.250 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.42.192.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:schoolcreate:computers</t>
   </si>
   <si>
     <t xml:space="preserve"># Rechnertyp</t>
@@ -158,35 +210,19 @@
     <t xml:space="preserve">windows</t>
   </si>
   <si>
-    <t xml:space="preserve">wing123m-01</t>
+    <t xml:space="preserve">win-042-001 </t>
   </si>
   <si>
     <t xml:space="preserve">10:00:ee:ﬀ:cc:00</t>
   </si>
   <si>
-    <t xml:space="preserve">g123m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.0.5.5</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:printers</t>
-    </r>
+    <t xml:space="preserve">123-456-789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edukativ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:printers</t>
   </si>
   <si>
     <t xml:space="preserve"># Aktion</t>
@@ -201,54 +237,103 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">dcg123m-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g123m-laserdrucker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">socket://10.0.5.250:9100</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:importusers</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Benutzername</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"># </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:classes</t>
-    </r>
+    <t xml:space="preserve">dru-042-012 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket://10.42.1.201:9100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:importusers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Vorname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nachname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schulen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somerville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">042-7a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e7c66ffb-afe1-4290-88df-948821b24876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mary@example.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lovelace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">042-6b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b998acd3-774c-4ccd-97b7-5fec820cc9c4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ada@example.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Susan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">042-5c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8ccc861f-652e-4f96-b796-aea2a7e827c8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skare@example.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margaret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamilton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a2eaab3f-e034-4df5-b66b-4610d24596d3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nasa@moon.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hopper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1ad9f83a-3473-41e3-9bb7-32af7ba74983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grace@hopper.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:classes</t>
   </si>
   <si>
     <t xml:space="preserve">Gruppen- / Klassenname</t>
@@ -270,6 +355,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -291,6 +377,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -335,7 +422,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,36 +431,44 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,18 +489,18 @@
       <c r="D2" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -419,22 +514,19 @@
       <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -449,59 +541,229 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>17</v>
+      <c r="A1" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:network:import" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:network:import"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:network:import" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:schoolcreate:network:import"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -510,79 +772,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.484693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>24</v>
+      <c r="A1" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>36</v>
+      <c r="F3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:computers" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:schoolcreate:computers"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:schoolcreate:computers" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:schoolcreate:computers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -591,70 +857,68 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>37</v>
+      <c r="A1" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>35</v>
+        <v>69</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>43</v>
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:printers" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:printers"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:printers" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:printers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -663,41 +927,154 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>45</v>
+      <c r="A1" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>74</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:importusers" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:importusers"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:importusers" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:importusers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -706,50 +1083,48 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>47</v>
+      <c r="A1" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:classes" display="https://docs.software-univention.de/ucsschool-handbuch-4.1R2.html#school:setup:cli:classes"/>
+    <hyperlink ref="A1" r:id="rId1" location="school:setup:cli:classes" display="# https://docs.software-univention.de/ucsschool-handbuch-4.4.html#school:setup:cli:classes"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>